<commit_message>
Update Pertanggal 2 Januari 2025 18:51 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Master.TblEducationalInstitution.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Master.TblEducationalInstitution.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
-    <sheet name="LookUp" sheetId="2" r:id="rId2"/>
+    <sheet name="DataLookUp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -443,14 +443,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -782,10 +775,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="B1:I9"/>
+  <dimension ref="B1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +868,7 @@
         <v>265000000000002</v>
       </c>
       <c r="I5" s="5" t="str">
-        <f t="shared" ref="I5:I8" si="0">IF(EXACT(B5, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-Master"".""Func_TblEducationalInstitution_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, '", B5, "'::varchar, ", IF(EXACT(C5, ""), "null::bigint", CONCATENATE(C5, "::bigint")), ", ", IF(EXACT(D5, ""), "null::varchar", CONCATENATE("'", D5, "'::varchar")), ", ", IF(EXACT(E5, ""), "null::bigint", CONCATENATE(E5, "::bigint")), ", ", IF(EXACT(F5, ""), "null::varchar", CONCATENATE("'", F5, "'::varchar")), ");"))</f>
+        <f t="shared" ref="I5:I7" si="0">IF(EXACT(B5, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-Master"".""Func_TblEducationalInstitution_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, '", B5, "'::varchar, ", IF(EXACT(C5, ""), "null::bigint", CONCATENATE(C5, "::bigint")), ", ", IF(EXACT(D5, ""), "null::varchar", CONCATENATE("'", D5, "'::varchar")), ", ", IF(EXACT(E5, ""), "null::bigint", CONCATENATE(E5, "::bigint")), ", ", IF(EXACT(F5, ""), "null::varchar", CONCATENATE("'", F5, "'::varchar")), ");"))</f>
         <v>PERFORM "SchData-OLTP-Master"."Func_TblEducationalInstitution_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 'SMPN 1 Padalarang'::varchar, 265000000000003::bigint, 'Jl. U.Suryadi No. 15'::varchar, null::bigint, null::varchar);</v>
       </c>
     </row>
@@ -924,56 +917,36 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="33"/>
-      <c r="H8" s="13">
-        <f xml:space="preserve"> H7 + IF(EXACT(I8, ""), 0, 1)</f>
-        <v>265000000000004</v>
-      </c>
-      <c r="I8" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="36"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12" t="str">
-        <f t="shared" ref="I5:I9" si="1">IF(EXACT(B9, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-Master"".""Func_TblEducationalInstitutionType_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, '", B9, "'::varchar);"))</f>
+      <c r="B8" s="4"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="36"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12" t="str">
+        <f t="shared" ref="I8" si="1">IF(EXACT(B8, ""), "", CONCATENATE("PERFORM ""SchData-OLTP-Master"".""Func_TblEducationalInstitutionType_SET""(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, '", B8, "'::varchar);"))</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>EXACT(H3, H4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>EXACT(H4, H5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>EXACT(H5, H6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>EXACT(H6, H7)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>EXACT(H7, H8)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -989,10 +962,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="B1:C9"/>
+  <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,22 +1029,12 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="B8" s="18" t="str">
         <f>IF(EXACT(MAIN!$H8, ""), "", MAIN!$H8)</f>
-        <v>265000000000004</v>
-      </c>
-      <c r="C8" s="17" t="str">
+        <v/>
+      </c>
+      <c r="C8" s="19" t="str">
         <f>IF(EXACT(MAIN!B8, ""), "", MAIN!B8)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="str">
-        <f>IF(EXACT(MAIN!$H9, ""), "", MAIN!$H9)</f>
-        <v/>
-      </c>
-      <c r="C9" s="19" t="str">
-        <f>IF(EXACT(MAIN!B9, ""), "", MAIN!B9)</f>
         <v/>
       </c>
     </row>

</xml_diff>